<commit_message>
fix: update roi calculate
</commit_message>
<xml_diff>
--- a/result/roi_calculate.xlsx
+++ b/result/roi_calculate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Programing\Python\Fomalhaut\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3538BC2A-CB7F-4041-940B-EFB9EBAFB94B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{800C2722-ECA8-49C7-A91B-AC8054E0A1FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-6000" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Die Hard 2</t>
   </si>
@@ -146,6 +146,18 @@
   </si>
   <si>
     <t>57,120,318</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>revenue</t>
+  </si>
+  <si>
+    <t>budget</t>
+  </si>
+  <si>
+    <t>roi</t>
   </si>
 </sst>
 </file>
@@ -521,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -537,211 +549,225 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>42</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>2.4290156285714279</v>
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>3.0202757076923081</v>
+        <v>2.4290156285714279</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>1.6320122166666671</v>
+        <v>3.0202757076923081</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D4">
-        <v>1.532704851851852</v>
+        <v>1.6320122166666671</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5">
-        <v>-0.17035586</v>
+        <v>1.532704851851852</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D6">
-        <v>-0.58319614285714283</v>
+        <v>-0.17035586</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D7">
-        <v>1.2072069361702129</v>
+        <v>-0.58319614285714283</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
         <v>20</v>
       </c>
       <c r="D8">
-        <v>-0.66614485106382981</v>
+        <v>1.2072069361702129</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="D9">
-        <v>1.8558656666666671</v>
+        <v>-0.66614485106382981</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D10">
-        <v>5.1131895749999998</v>
+        <v>1.8558656666666671</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C11" t="s">
         <v>28</v>
       </c>
       <c r="D11">
-        <v>-0.76892150000000004</v>
+        <v>5.1131895749999998</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D12">
-        <v>3.0399729999999998</v>
+        <v>-0.76892150000000004</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D13">
-        <v>0.25046692678811527</v>
+        <v>3.0399729999999998</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D14">
-        <v>0.3051763714285714</v>
+        <v>0.25046692678811527</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C15" t="s">
         <v>39</v>
       </c>
       <c r="D15">
+        <v>0.3051763714285714</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D16">
         <v>0.63200908571428571</v>
       </c>
     </row>

</xml_diff>